<commit_message>
Check Prisma guidelines for submission
</commit_message>
<xml_diff>
--- a/submission/prisma_checklist.xlsx
+++ b/submission/prisma_checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\literature_review\submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232E089C-1B7C-4F22-849F-FB89BB771AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C93EC7-7369-4AFE-8B1F-F528D6222C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22860" yWindow="-20715" windowWidth="21600" windowHeight="11385" xr2:uid="{4E9F63C3-EBA8-4194-8BB8-6578E5E7EB9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4E9F63C3-EBA8-4194-8BB8-6578E5E7EB9C}"/>
   </bookViews>
   <sheets>
     <sheet name="abstract checklist" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="123">
   <si>
     <t>Section and topic</t>
   </si>
@@ -394,14 +394,23 @@
     <t>not applicable</t>
   </si>
   <si>
-    <t>not into the abstract, but discussion</t>
+    <t>Checked?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Topic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,22 +424,27 @@
       <name val="CMU Serif"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="CMU Serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="CMU Serif"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -438,11 +452,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -462,18 +491,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -783,217 +833,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F661DC-2F15-416B-846F-AA32B213CE10}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="104.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="66" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8">
+      <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="E2" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="132" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8">
+      <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="E3" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C4" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8">
+      <c r="C5" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="99" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="E5" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C6" s="9">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E6" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="99" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="7" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C7" s="9">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="E7" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="165" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8">
+      <c r="C8" s="9">
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="E8" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8">
+      <c r="C9" s="9">
         <v>8</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="9">
+        <v>9</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="9">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="9">
+        <v>11</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9">
+        <v>12</v>
+      </c>
       <c r="D13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="214.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="8">
-        <v>9</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="8">
-        <v>10</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="8">
-        <v>11</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="8">
-        <v>12</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>118</v>
-      </c>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="yes">
+      <formula>NOT(ISERROR(SEARCH("yes",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>